<commit_message>
Add data comparison for all sections. Data now loads from excel files.
</commit_message>
<xml_diff>
--- a/ExcelFiles/ReferralPortal.xlsx
+++ b/ExcelFiles/ReferralPortal.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Riomed\Cellma4Automation\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA7A057-B0E4-4A30-8993-AC4F99427733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49253F09-1CF0-4D63-BC2D-8C345A68E970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="loginDetails" sheetId="1" r:id="rId1"/>
     <sheet name="patientDetails" sheetId="2" r:id="rId2"/>
     <sheet name="referralDetails" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="conditionDetails" sheetId="4" r:id="rId4"/>
+    <sheet name="medicationDetails" sheetId="5" r:id="rId5"/>
+    <sheet name="investigationDetails" sheetId="6" r:id="rId6"/>
+    <sheet name="patientScanDetails" sheetId="7" r:id="rId7"/>
+    <sheet name="procedureDetails" sheetId="8" r:id="rId8"/>
+    <sheet name="referralDocuments" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="153">
   <si>
     <t>username</t>
   </si>
@@ -149,22 +154,355 @@
     <t>RioMed Demosite</t>
   </si>
   <si>
-    <t>Cardiology Ward</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mr Dhanashree Abnavea </t>
   </si>
   <si>
-    <t>Brittany</t>
-  </si>
-  <si>
-    <t>09/12/1989</t>
-  </si>
-  <si>
-    <t>801238493</t>
-  </si>
-  <si>
-    <t>hospRef1012</t>
+    <t>ANA Location</t>
+  </si>
+  <si>
+    <t>Note has been added for testing</t>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>cond_record_status</t>
+  </si>
+  <si>
+    <t>cond_notes</t>
+  </si>
+  <si>
+    <t>cond_previous</t>
+  </si>
+  <si>
+    <t>cond_date_diagnosed</t>
+  </si>
+  <si>
+    <t>06/12/2024</t>
+  </si>
+  <si>
+    <t>pacr_category</t>
+  </si>
+  <si>
+    <t>pacr_que_name</t>
+  </si>
+  <si>
+    <t>Hypertension</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Dental</t>
+  </si>
+  <si>
+    <t>Medication addition test.</t>
+  </si>
+  <si>
+    <t>Increased dose</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>produced</t>
+  </si>
+  <si>
+    <t>Test Method</t>
+  </si>
+  <si>
+    <t>continuous</t>
+  </si>
+  <si>
+    <t>medi_route</t>
+  </si>
+  <si>
+    <t>medi_notes</t>
+  </si>
+  <si>
+    <t>medi_stopped_reason_eli_text</t>
+  </si>
+  <si>
+    <t>medi_prescribed_by</t>
+  </si>
+  <si>
+    <t>medi_status</t>
+  </si>
+  <si>
+    <t>medi_stop_date</t>
+  </si>
+  <si>
+    <t>medi_start_date</t>
+  </si>
+  <si>
+    <t>medi_duration</t>
+  </si>
+  <si>
+    <t>medi_method</t>
+  </si>
+  <si>
+    <t>medi_frequency</t>
+  </si>
+  <si>
+    <t>medi_dose</t>
+  </si>
+  <si>
+    <t>inv_status</t>
+  </si>
+  <si>
+    <t>inv_notes</t>
+  </si>
+  <si>
+    <t>inv_for_imaging</t>
+  </si>
+  <si>
+    <t>inv_for_labrequest</t>
+  </si>
+  <si>
+    <t>inv_completed</t>
+  </si>
+  <si>
+    <t>inv_review_date</t>
+  </si>
+  <si>
+    <t>inv_risk</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Investigation notes test entry</t>
+  </si>
+  <si>
+    <t>inv_status_entry</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>pascn_t_score</t>
+  </si>
+  <si>
+    <t>pascn_z_score</t>
+  </si>
+  <si>
+    <t>pascn_bmd_score</t>
+  </si>
+  <si>
+    <t>pascn_machine_name</t>
+  </si>
+  <si>
+    <t>pascn_site_name</t>
+  </si>
+  <si>
+    <t>pascn_scan_type_eli_text</t>
+  </si>
+  <si>
+    <t>pascn_scan_date</t>
+  </si>
+  <si>
+    <t>pascn_scan_result</t>
+  </si>
+  <si>
+    <t>pascn_risk</t>
+  </si>
+  <si>
+    <t>pascn_notes</t>
+  </si>
+  <si>
+    <t>Ultrasound</t>
+  </si>
+  <si>
+    <t>Hip and Spine</t>
+  </si>
+  <si>
+    <t>CT Scan</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Patient scan data entry test</t>
+  </si>
+  <si>
+    <t>Patient Scan</t>
+  </si>
+  <si>
+    <t>Heel DEXA scan</t>
+  </si>
+  <si>
+    <t>proc_risk</t>
+  </si>
+  <si>
+    <t>proc_outcome</t>
+  </si>
+  <si>
+    <t>proc_status</t>
+  </si>
+  <si>
+    <t>proc_procedure_date</t>
+  </si>
+  <si>
+    <t>proc_completed_date</t>
+  </si>
+  <si>
+    <t>proc_site</t>
+  </si>
+  <si>
+    <t>proc_type</t>
+  </si>
+  <si>
+    <t>proc_procedure_level</t>
+  </si>
+  <si>
+    <t>proc_notes</t>
+  </si>
+  <si>
+    <t>abnormal</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>tertiary</t>
+  </si>
+  <si>
+    <t>Procedure data entry test</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Lymphadenectomy</t>
+  </si>
+  <si>
+    <t>doc_category</t>
+  </si>
+  <si>
+    <t>doc_description</t>
+  </si>
+  <si>
+    <t>doc_to</t>
+  </si>
+  <si>
+    <t>doc_original_name</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Referral Document data entry test</t>
+  </si>
+  <si>
+    <t>PatientPic.png</t>
+  </si>
+  <si>
+    <t>refd_additional_notes</t>
+  </si>
+  <si>
+    <t>Additional information of the referral data entry test</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Atenolol 10mg tablets</t>
+  </si>
+  <si>
+    <t>medi_site</t>
+  </si>
+  <si>
+    <t>Bilateral</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>19/12/2024</t>
+  </si>
+  <si>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>mse_text</t>
+  </si>
+  <si>
+    <t>sickness</t>
+  </si>
+  <si>
+    <t>medi_status_entry</t>
+  </si>
+  <si>
+    <t>Produced</t>
+  </si>
+  <si>
+    <t>Liver Function Test</t>
+  </si>
+  <si>
+    <t>Investigation</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>24/12/2024</t>
+  </si>
+  <si>
+    <t>23/12/2024</t>
+  </si>
+  <si>
+    <t>30/12/2024</t>
+  </si>
+  <si>
+    <t>proc_type_entry</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>proc_procedure_level_entry</t>
+  </si>
+  <si>
+    <t>Tertiary</t>
+  </si>
+  <si>
+    <t>proc_outcome_entry</t>
+  </si>
+  <si>
+    <t>proc_status_entry</t>
+  </si>
+  <si>
+    <t>Abnormal</t>
+  </si>
+  <si>
+    <t>proc_site_entry</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>Violet</t>
+  </si>
+  <si>
+    <t>09/12/2000</t>
+  </si>
+  <si>
+    <t>801638493</t>
+  </si>
+  <si>
+    <t>hospRef1016</t>
   </si>
 </sst>
 </file>
@@ -206,12 +544,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +919,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -591,13 +932,13 @@
         <v>F</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>150</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="H2" t="s">
         <v>34</v>
@@ -610,28 +951,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81CC3426-46CB-48C6-AE92-29ADF8DD389A}">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="9.90625" customWidth="1"/>
+    <col min="3" max="3" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="46.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -671,8 +1015,11 @@
       <c r="M1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -683,17 +1030,17 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E2" t="str">
         <f ca="1">TEXT(TODAY(),"dd/mm/yyyy")</f>
-        <v>06/01/2025</v>
+        <v>10/01/2025</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
         <v>19</v>
@@ -713,6 +1060,9 @@
       </c>
       <c r="M2" t="s">
         <v>26</v>
+      </c>
+      <c r="N2" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -723,12 +1073,573 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B1556-9305-4DB0-A484-EA49D36DADC5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08A8DDCC-4A6A-4CF6-AC25-3E373653A611}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P1" sqref="O1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.54296875" customWidth="1"/>
+    <col min="15" max="15" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>122</v>
+      </c>
+      <c r="N1" t="s">
+        <v>128</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>51</v>
+      </c>
+      <c r="L2" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N2" t="s">
+        <v>129</v>
+      </c>
+      <c r="O2" t="s">
+        <v>120</v>
+      </c>
+      <c r="P2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0449301-D87B-42F1-9FAE-92EDDB978788}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s">
+        <v>133</v>
+      </c>
+      <c r="J2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D238D5CA-0202-4C30-86F5-794286AC32BB}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41707E3A-B1B5-448A-B242-C36FF4E43C39}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.36328125" customWidth="1"/>
+    <col min="10" max="10" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="19.7265625" customWidth="1"/>
+    <col min="14" max="14" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I1" t="s">
+        <v>139</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="N1" t="s">
+        <v>104</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+      <c r="L2" t="s">
+        <v>148</v>
+      </c>
+      <c r="M2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" t="s">
+        <v>109</v>
+      </c>
+      <c r="P2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B706C8B-9B59-4AD5-BE52-84611DB0D786}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="str">
+        <f>referralDetails!G2</f>
+        <v xml:space="preserve">Mr Dhanashree Abnavea </v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>